<commit_message>
a function for every source of economic data
</commit_message>
<xml_diff>
--- a/data/interim/economical/calibration_data/ERMG_revenue_survey.xlsx
+++ b/data/interim/economical/calibration_data/ERMG_revenue_survey.xlsx
@@ -211,7 +211,7 @@
     <t xml:space="preserve">97-98</t>
   </si>
   <si>
-    <t xml:space="preserve">Belgium</t>
+    <t xml:space="preserve">BE</t>
   </si>
 </sst>
 </file>
@@ -328,11 +328,11 @@
   </sheetPr>
   <dimension ref="A1:X65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A66" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="1" style="0" width="9.07"/>
   </cols>
@@ -3202,8 +3202,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>